<commit_message>
Update smoothing time for electricity price changes to 20
</commit_message>
<xml_diff>
--- a/InputData/elec/STfEPC/STfEPC Smoothing Time for Electricity Price Changes.xlsx
+++ b/InputData/elec/STfEPC/STfEPC Smoothing Time for Electricity Price Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\STfEPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6D79CD-36F5-4AA8-93C7-69BDF9195725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBBC99A-59FA-4864-A9A7-EE0BDD725E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -631,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="9">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>

</xml_diff>

<commit_message>
Change one variable name and tweak depreciation times in preparation for adding financing of elec sector capital eqpt.
</commit_message>
<xml_diff>
--- a/InputData/elec/STfEPC/STfEPC Smoothing Time for Electricity Price Changes.xlsx
+++ b/InputData/elec/STfEPC/STfEPC Smoothing Time for Electricity Price Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\STfEPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E18E19-2506-428A-A4C4-BEE78DA96BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAC34D1-7655-4860-9EAA-39112E9B28DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12075" yWindow="450" windowWidth="33855" windowHeight="21540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12420" yWindow="795" windowWidth="33855" windowHeight="21540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>